<commit_message>
Fixed blackout date and last facility inspection date. (Need to to change color for today's date in template)
</commit_message>
<xml_diff>
--- a/ALF_Scheduler/Copy of UpdatedTestData.xlsx
+++ b/ALF_Scheduler/Copy of UpdatedTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Homework\ALFCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mical\source\repos\KennethWhite\ALF_Scheduler\ALF_Scheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00A681FB-9DB4-416E-8FA4-54D5CA87BE51}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5653CEF-23BC-4AD7-9F9A-F228E5C33B91}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2715" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -938,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:S10"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1590,29 +1590,29 @@
         <v>31</v>
       </c>
       <c r="G10" s="23">
-        <v>42209</v>
+        <v>42575</v>
       </c>
       <c r="H10" s="23">
-        <v>42594</v>
+        <v>43171</v>
       </c>
       <c r="I10" s="22">
         <f t="shared" si="0"/>
-        <v>12.664473684210527</v>
+        <v>19.605263157894736</v>
       </c>
       <c r="J10" s="22">
         <f t="shared" si="1"/>
-        <v>385</v>
+        <v>596</v>
       </c>
       <c r="K10" s="23">
         <v>43507</v>
       </c>
       <c r="L10" s="23">
         <f t="shared" si="2"/>
-        <v>43111</v>
+        <v>43688</v>
       </c>
       <c r="M10" s="23">
         <f t="shared" si="3"/>
-        <v>43141.2</v>
+        <v>43718.2</v>
       </c>
       <c r="N10" s="22" t="s">
         <v>73</v>

</xml_diff>